<commit_message>
Fix temperature conversion check, had caused temp conversion error, v1.5
</commit_message>
<xml_diff>
--- a/unit-converter.xlsx
+++ b/unit-converter.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sasha\Git-repos\unit-converter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sasha\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A30C500-9B89-41A4-874A-03CFA90EBDD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A001FD43-FBA5-49CE-B838-D3F34D890562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1445,9 +1445,6 @@
     <t>https://physics.nist.gov/cgi-bin/cuu/Value?c</t>
   </si>
   <si>
-    <t>Version: 1.4</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -1466,6 +1463,9 @@
       </rPr>
       <t xml:space="preserve"> https://github.com/sashahafner/unit-converter/</t>
     </r>
+  </si>
+  <si>
+    <t>Version: 1.5</t>
   </si>
 </sst>
 </file>
@@ -1642,7 +1642,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1783,15 +1783,6 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
@@ -1800,26 +1791,20 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2259,34 +2244,34 @@
       <c r="L8" s="36"/>
     </row>
     <row r="9" spans="4:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="51" t="s">
+      <c r="D9" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="51"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="51"/>
-      <c r="L9" s="51"/>
-      <c r="M9" s="51"/>
-      <c r="N9" s="51"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="54"/>
+      <c r="L9" s="54"/>
+      <c r="M9" s="54"/>
+      <c r="N9" s="54"/>
     </row>
     <row r="11" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D11" s="52" t="s">
+      <c r="D11" s="55" t="s">
         <v>174</v>
       </c>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="52"/>
-      <c r="K11" s="52"/>
-      <c r="L11" s="52"/>
-      <c r="M11" s="52"/>
-      <c r="N11" s="52"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="55"/>
+      <c r="H11" s="55"/>
+      <c r="I11" s="55"/>
+      <c r="J11" s="55"/>
+      <c r="K11" s="55"/>
+      <c r="L11" s="55"/>
+      <c r="M11" s="55"/>
+      <c r="N11" s="55"/>
     </row>
     <row r="12" spans="4:14" ht="4.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="4:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2335,16 +2320,14 @@
       <c r="D15" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="30">
-        <v>1</v>
-      </c>
+      <c r="E15" s="30"/>
       <c r="F15" s="38" t="s">
         <v>176</v>
       </c>
-      <c r="G15" s="54" t="s">
+      <c r="G15" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="H15" s="55" t="s">
+      <c r="H15" s="52" t="s">
         <v>7</v>
       </c>
       <c r="I15" s="46" t="s">
@@ -2419,19 +2402,19 @@
       <c r="N19" s="40"/>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D21" s="52" t="s">
+      <c r="D21" s="55" t="s">
         <v>175</v>
       </c>
-      <c r="E21" s="52"/>
-      <c r="F21" s="52"/>
-      <c r="G21" s="52"/>
-      <c r="H21" s="52"/>
-      <c r="I21" s="52"/>
-      <c r="J21" s="52"/>
-      <c r="K21" s="52"/>
-      <c r="L21" s="52"/>
-      <c r="M21" s="52"/>
-      <c r="N21" s="52"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="55"/>
+      <c r="H21" s="55"/>
+      <c r="I21" s="55"/>
+      <c r="J21" s="55"/>
+      <c r="K21" s="55"/>
+      <c r="L21" s="55"/>
+      <c r="M21" s="55"/>
+      <c r="N21" s="55"/>
     </row>
     <row r="22" spans="3:14" ht="4.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="23" spans="3:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2490,7 +2473,7 @@
       <c r="G25" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="H25" s="47" t="s">
+      <c r="H25" s="52" t="s">
         <v>7</v>
       </c>
       <c r="I25" s="46" t="s">
@@ -2544,17 +2527,17 @@
     </row>
     <row r="34" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D34" s="35" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="35" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D35" s="56" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="35" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D35" s="62" t="s">
-        <v>354</v>
-      </c>
-      <c r="E35" s="62"/>
-      <c r="F35" s="62"/>
-      <c r="G35" s="62"/>
-      <c r="H35" s="62"/>
+      <c r="E35" s="56"/>
+      <c r="F35" s="56"/>
+      <c r="G35" s="56"/>
+      <c r="H35" s="56"/>
     </row>
     <row r="92" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D92" s="38" t="s">
@@ -2737,34 +2720,34 @@
       <c r="L8" s="36"/>
     </row>
     <row r="9" spans="4:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="51" t="s">
+      <c r="D9" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="51"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="51"/>
-      <c r="L9" s="51"/>
-      <c r="M9" s="51"/>
-      <c r="N9" s="51"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="54"/>
+      <c r="L9" s="54"/>
+      <c r="M9" s="54"/>
+      <c r="N9" s="54"/>
     </row>
     <row r="11" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D11" s="52" t="s">
+      <c r="D11" s="55" t="s">
         <v>174</v>
       </c>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="52"/>
-      <c r="J11" s="52"/>
-      <c r="K11" s="52"/>
-      <c r="L11" s="52"/>
-      <c r="M11" s="52"/>
-      <c r="N11" s="52"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="55"/>
+      <c r="H11" s="55"/>
+      <c r="I11" s="55"/>
+      <c r="J11" s="55"/>
+      <c r="K11" s="55"/>
+      <c r="L11" s="55"/>
+      <c r="M11" s="55"/>
+      <c r="N11" s="55"/>
     </row>
     <row r="12" spans="4:14" ht="4.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="4:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2897,19 +2880,19 @@
       <c r="N19" s="40"/>
     </row>
     <row r="20" spans="4:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D20" s="52" t="s">
+      <c r="D20" s="55" t="s">
         <v>218</v>
       </c>
-      <c r="E20" s="52"/>
-      <c r="F20" s="52"/>
-      <c r="G20" s="52"/>
-      <c r="H20" s="52"/>
-      <c r="I20" s="52"/>
-      <c r="J20" s="52"/>
-      <c r="K20" s="52"/>
-      <c r="L20" s="52"/>
-      <c r="M20" s="52"/>
-      <c r="N20" s="52"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="55"/>
+      <c r="I20" s="55"/>
+      <c r="J20" s="55"/>
+      <c r="K20" s="55"/>
+      <c r="L20" s="55"/>
+      <c r="M20" s="55"/>
+      <c r="N20" s="55"/>
     </row>
     <row r="21" spans="4:14" ht="4.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="22" spans="4:14" x14ac:dyDescent="0.2">
@@ -2962,19 +2945,19 @@
       </c>
     </row>
     <row r="29" spans="4:14" x14ac:dyDescent="0.2">
-      <c r="D29" s="52" t="s">
+      <c r="D29" s="55" t="s">
         <v>175</v>
       </c>
-      <c r="E29" s="52"/>
-      <c r="F29" s="52"/>
-      <c r="G29" s="52"/>
-      <c r="H29" s="52"/>
-      <c r="I29" s="52"/>
-      <c r="J29" s="52"/>
-      <c r="K29" s="52"/>
-      <c r="L29" s="52"/>
-      <c r="M29" s="52"/>
-      <c r="N29" s="52"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="55"/>
+      <c r="I29" s="55"/>
+      <c r="J29" s="55"/>
+      <c r="K29" s="55"/>
+      <c r="L29" s="55"/>
+      <c r="M29" s="55"/>
+      <c r="N29" s="55"/>
     </row>
     <row r="30" spans="4:14" ht="4.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="31" spans="4:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3133,405 +3116,405 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="13.42578125" style="57" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" style="57" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" style="57" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" style="57" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="57"/>
+    <col min="1" max="2" width="13.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="57" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
         <v>220</v>
       </c>
-      <c r="B1" s="56"/>
-    </row>
-    <row r="2" spans="1:4" s="59" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="58" t="s">
+      <c r="B1" s="18"/>
+    </row>
+    <row r="2" spans="1:4" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="C2" s="58" t="s">
+      <c r="C2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="58" t="s">
+      <c r="D2" s="4" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="59" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="59" t="s">
+    <row r="3" spans="1:4" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="60">
+      <c r="B3" s="14">
         <f t="shared" ref="B3:B27" si="0">CODE(A3)</f>
         <v>46</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="D3" s="59">
+      <c r="D3" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="59" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="59" t="s">
+    <row r="4" spans="1:4" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="B4" s="60">
+      <c r="B4" s="14">
         <f t="shared" si="0"/>
         <v>81</v>
       </c>
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="D4" s="59">
+      <c r="D4" s="2">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="59" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="59" t="s">
+    <row r="5" spans="1:4" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="B5" s="60">
+      <c r="B5" s="14">
         <f t="shared" si="0"/>
         <v>82</v>
       </c>
-      <c r="C5" s="59" t="s">
+      <c r="C5" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="D5" s="59">
+      <c r="D5" s="2">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="57" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="57" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="B6" s="60">
+      <c r="B6" s="14">
         <f t="shared" si="0"/>
         <v>89</v>
       </c>
-      <c r="C6" s="57" t="s">
+      <c r="C6" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D6" s="61">
+      <c r="D6" s="53">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="57" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="57" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="B7" s="60">
+      <c r="B7" s="14">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="C7" s="57" t="s">
+      <c r="C7" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D7" s="61">
+      <c r="D7" s="53">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="57" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="57" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="60">
+      <c r="B8" s="14">
         <f t="shared" si="0"/>
         <v>69</v>
       </c>
-      <c r="C8" s="57" t="s">
+      <c r="C8" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="61">
+      <c r="D8" s="53">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="57" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="57" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="60">
+      <c r="B9" s="14">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="C9" s="57" t="s">
+      <c r="C9" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="61">
+      <c r="D9" s="53">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="57" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="57" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B10" s="60">
+      <c r="B10" s="14">
         <f t="shared" si="0"/>
         <v>84</v>
       </c>
-      <c r="C10" s="57" t="s">
+      <c r="C10" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D10" s="61">
+      <c r="D10" s="53">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="57" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="57" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B11" s="60">
+      <c r="B11" s="14">
         <f t="shared" si="0"/>
         <v>71</v>
       </c>
-      <c r="C11" s="57" t="s">
+      <c r="C11" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D11" s="61">
+      <c r="D11" s="53">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="57" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="57" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B12" s="60">
+      <c r="B12" s="14">
         <f t="shared" si="0"/>
         <v>77</v>
       </c>
-      <c r="C12" s="57" t="s">
+      <c r="C12" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D12" s="61">
+      <c r="D12" s="53">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="57" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="57" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B13" s="60">
+      <c r="B13" s="14">
         <f t="shared" si="0"/>
         <v>107</v>
       </c>
-      <c r="C13" s="57" t="s">
+      <c r="C13" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D13" s="61">
+      <c r="D13" s="53">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="57" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="57" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B14" s="60">
+      <c r="B14" s="14">
         <f t="shared" si="0"/>
         <v>104</v>
       </c>
-      <c r="C14" s="57" t="s">
+      <c r="C14" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D14" s="61">
+      <c r="D14" s="53">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="57" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="57" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B15" s="60">
+      <c r="B15" s="14">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="C15" s="57" t="s">
+      <c r="C15" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="61">
+      <c r="D15" s="53">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="57" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="57" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="60">
+      <c r="B16" s="14">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="C16" s="57" t="s">
+      <c r="C16" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D16" s="61">
+      <c r="D16" s="53">
         <v>-1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="57" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="57" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B17" s="60">
+      <c r="B17" s="14">
         <f t="shared" si="0"/>
         <v>99</v>
       </c>
-      <c r="C17" s="57" t="s">
+      <c r="C17" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D17" s="61">
+      <c r="D17" s="53">
         <v>-2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="57" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="57" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="60">
+      <c r="B18" s="14">
         <f t="shared" si="0"/>
         <v>109</v>
       </c>
-      <c r="C18" s="57" t="s">
+      <c r="C18" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D18" s="61">
+      <c r="D18" s="53">
         <v>-3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="57" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="57" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B19" s="60">
+      <c r="B19" s="14">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="C19" s="57" t="s">
+      <c r="C19" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D19" s="61">
+      <c r="D19" s="53">
         <v>-6</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="57" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="57" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="60">
+      <c r="B20" s="14">
         <f t="shared" si="0"/>
         <v>110</v>
       </c>
-      <c r="C20" s="57" t="s">
+      <c r="C20" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D20" s="61">
+      <c r="D20" s="53">
         <v>-9</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="57" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="57" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="B21" s="60">
+      <c r="B21" s="14">
         <f t="shared" si="0"/>
         <v>112</v>
       </c>
-      <c r="C21" s="57" t="s">
+      <c r="C21" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D21" s="61">
+      <c r="D21" s="53">
         <v>-12</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="57" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="57" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B22" s="60">
+      <c r="B22" s="14">
         <f t="shared" si="0"/>
         <v>102</v>
       </c>
-      <c r="C22" s="57" t="s">
+      <c r="C22" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D22" s="61">
+      <c r="D22" s="53">
         <v>-15</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="57" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="57" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B23" s="60">
+      <c r="B23" s="14">
         <f t="shared" si="0"/>
         <v>97</v>
       </c>
-      <c r="C23" s="57" t="s">
+      <c r="C23" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D23" s="61">
+      <c r="D23" s="53">
         <v>-18</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="57" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="57" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="B24" s="60">
+      <c r="B24" s="14">
         <f t="shared" si="0"/>
         <v>122</v>
       </c>
-      <c r="C24" s="57" t="s">
+      <c r="C24" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D24" s="61">
+      <c r="D24" s="53">
         <v>-21</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="57" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="57" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="B25" s="60">
+      <c r="B25" s="14">
         <f t="shared" si="0"/>
         <v>121</v>
       </c>
-      <c r="C25" s="57" t="s">
+      <c r="C25" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D25" s="61">
+      <c r="D25" s="53">
         <v>-24</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="57" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="57" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="B26" s="60">
+      <c r="B26" s="14">
         <f t="shared" si="0"/>
         <v>114</v>
       </c>
-      <c r="C26" s="57" t="s">
+      <c r="C26" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="D26" s="61">
+      <c r="D26" s="53">
         <v>-27</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="57" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="57" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="B27" s="60">
+      <c r="B27" s="14">
         <f t="shared" si="0"/>
         <v>113</v>
       </c>
-      <c r="C27" s="57" t="s">
+      <c r="C27" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="D27" s="61">
+      <c r="D27" s="53">
         <v>-30</v>
       </c>
     </row>
@@ -5708,10 +5691,10 @@
       <c r="G2" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
     </row>
     <row r="3" spans="1:12" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -6723,7 +6706,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6841,7 +6824,7 @@
         <v>224</v>
       </c>
       <c r="B10" s="5">
-        <f>IF(AND(Regular!J15=".",Regular!L15=".",Regular!N15=".",Regular!H24=".",Regular!J24=".",Regular!L24=".",Regular!J25=".",Regular!L25=".",Regular!N25=".",VLOOKUP(Regular!H15,F!A3:G78,7,FALSE)=D!D7,VLOOKUP(Regular!H25,F!A3:G78,7,FALSE)=D!D7),1,0)</f>
+        <f>IF(AND(Regular!J15=".",Regular!L15=".",Regular!N15=".",Regular!J25=".",Regular!L25=".",Regular!N25=".",VLOOKUP(Regular!H15,F!A3:G78,7,FALSE)=D!D7,VLOOKUP(Regular!H25,F!A3:G78,7,FALSE)=D!D7),1,0)</f>
         <v>0</v>
       </c>
       <c r="C10" t="str">
@@ -7046,7 +7029,7 @@
       </c>
       <c r="B2" s="25">
         <f>Regular!E15*(10^VLOOKUP(CODE(Regular!G15),S!B3:D27,3,FALSE))^Regular!H14*(10^VLOOKUP(CODE(Regular!I15),S!B3:D27,3,FALSE))^Regular!J14*(10^VLOOKUP(CODE(Regular!K15),S!B3:D27,3,FALSE))^Regular!L14*(10^VLOOKUP(CODE(Regular!M15),S!B3:D27,3,FALSE))^Regular!N14*(10^VLOOKUP(CODE(Regular!G25),S!B3:D27,3,FALSE))^(-Regular!H24)*(10^VLOOKUP(CODE(Regular!I25),S!B3:D27,3,FALSE))^(-Regular!J24)*(10^VLOOKUP(CODE(Regular!K25),S!B3:D27,3,FALSE))^(-Regular!L24)*(10^VLOOKUP(CODE(Regular!M25),S!B3:D27,3,FALSE))^(-Regular!N24)*VLOOKUP(Regular!H15,F!A3:D78,4,FALSE)^Regular!H14*VLOOKUP(Regular!J15,F!A3:D78,4,FALSE)^Regular!J14*VLOOKUP(Regular!L15,F!A3:D78,4,FALSE)^Regular!L14*VLOOKUP(Regular!N15,F!A3:D78,4,FALSE)^Regular!N14*VLOOKUP(Regular!H25,F!A3:D78,4,FALSE)^(-Regular!H24)*VLOOKUP(Regular!J25,F!A3:D78,4,FALSE)^(-Regular!J24)*VLOOKUP(Regular!L25,F!A3:D78,4,FALSE)^(-Regular!L24)*VLOOKUP(Regular!N25,F!A3:D78,4,FALSE)^(-Regular!N24)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>